<commit_message>
UPDATE: Parses selected row/column/range and selected sheet
</commit_message>
<xml_diff>
--- a/xlsx/tests/example.xlsx
+++ b/xlsx/tests/example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20368"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nhatcher/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1735EC9-FFED-419C-B07A-CFF93E3E2AA9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E08456FE-9C8A-184E-905A-1DA5ECA32BA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="6020" windowHeight="50" activeTab="2" xr2:uid="{94D94FA5-4B40-4032-9EB1-15E3426A29B1}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" activeTab="8" xr2:uid="{94D94FA5-4B40-4032-9EB1-15E3426A29B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,9 @@
     <sheet name="Table" sheetId="7" r:id="rId6"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId7"/>
     <sheet name="Created fourth" sheetId="4" r:id="rId8"/>
-    <sheet name="Hidden" sheetId="5" state="hidden" r:id="rId9"/>
+    <sheet name="Frozen" sheetId="10" r:id="rId9"/>
+    <sheet name="Split" sheetId="11" r:id="rId10"/>
+    <sheet name="Hidden" sheetId="5" state="hidden" r:id="rId11"/>
   </sheets>
   <definedNames>
     <definedName name="answer" localSheetId="4">shared!$G$5</definedName>
@@ -32,11 +34,22 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId10"/>
+    <pivotCache cacheId="2" r:id="rId12"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -56,7 +69,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>nicol:</t>
         </r>
@@ -65,7 +78,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 This cell has bold! Text. Náguara!</t>
@@ -78,21 +91,30 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>nicol:</t>
         </r>
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-There is a coment here, you know
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">There is a coment here, you know
 </t>
         </r>
       </text>
@@ -105,7 +127,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>nicol:</t>
         </r>
@@ -114,7 +136,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 New comment</t>
@@ -129,7 +151,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>nicol:</t>
         </r>
@@ -138,7 +160,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 There is a </t>
@@ -158,7 +180,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> here.
 </t>
@@ -193,7 +215,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="47">
   <si>
     <t>A string</t>
   </si>
@@ -344,12 +366,27 @@
   <si>
     <t>With a tint</t>
   </si>
+  <si>
+    <t>Corner</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>B4</t>
+  </si>
+  <si>
+    <t>as</t>
+  </si>
+  <si>
+    <t>df</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -406,14 +443,14 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -437,20 +474,27 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="5" tint="-0.24994659260841701"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="36">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -659,6 +703,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="14">
     <border>
@@ -818,9 +880,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -832,7 +894,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
@@ -842,8 +903,41 @@
     <xf numFmtId="0" fontId="11" fillId="7" borderId="3" xfId="2"/>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="4" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="5" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="3" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="3" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -874,36 +968,6 @@
     <xf numFmtId="0" fontId="11" fillId="7" borderId="13" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="27" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="30" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Input" xfId="2" builtinId="20"/>
@@ -935,7 +999,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1276,7 +1340,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2827,7 +2891,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D44FF134-98CE-4CDD-8BF9-3EB1A09B9FAE}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D44FF134-98CE-4CDD-8BF9-3EB1A09B9FAE}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B13" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" showAll="0">
@@ -2924,9 +2988,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2964,7 +3028,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -3070,7 +3134,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3212,7 +3276,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3223,17 +3287,17 @@
   <dimension ref="A1:O33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="E13" sqref="E13:N20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="5" width="38.26953125" customWidth="1"/>
-    <col min="6" max="6" width="9.1796875" style="1"/>
+    <col min="5" max="5" width="38.33203125" customWidth="1"/>
+    <col min="6" max="6" width="9.1640625" style="1"/>
     <col min="8" max="8" width="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3254,7 +3318,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>222</v>
       </c>
@@ -3272,7 +3336,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B3">
         <f>A3</f>
         <v>0</v>
@@ -3288,44 +3352,44 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="I6" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="13" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="K7" s="17" t="s">
+    <row r="7" spans="1:15" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K7" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="L7" s="17"/>
-    </row>
-    <row r="8" spans="1:15" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="K8" s="17"/>
-      <c r="L8" s="17"/>
+      <c r="L7" s="49"/>
+    </row>
+    <row r="8" spans="1:15" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K8" s="49"/>
+      <c r="L8" s="49"/>
       <c r="N8" s="3"/>
       <c r="O8" s="3"/>
     </row>
-    <row r="9" spans="1:15" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" ht="29.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E9" t="s">
         <v>12</v>
       </c>
-      <c r="K9" s="17"/>
-      <c r="L9" s="17"/>
+      <c r="K9" s="49"/>
+      <c r="L9" s="49"/>
       <c r="N9" s="3" t="s">
         <v>8</v>
       </c>
       <c r="O9" s="3"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="K10" s="17"/>
-      <c r="L10" s="17"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="K10" s="49"/>
+      <c r="L10" s="49"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C14" t="s">
         <v>9</v>
       </c>
@@ -3334,24 +3398,24 @@
         <v>quantum</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="21" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="K15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2</v>
       </c>
-      <c r="H16" s="12"/>
-    </row>
-    <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H16" s="11"/>
+    </row>
+    <row r="17" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>6</v>
       </c>
-      <c r="H17" s="14"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H17" s="13"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>7</v>
       </c>
@@ -3359,36 +3423,36 @@
         <f>SUM(numbers)</f>
         <v>15</v>
       </c>
-      <c r="H18" s="18">
+      <c r="H18" s="50">
         <v>1</v>
       </c>
-      <c r="I18" s="19"/>
-      <c r="J18" s="20"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="H19" s="21"/>
-      <c r="I19" s="22"/>
-      <c r="J19" s="23"/>
-    </row>
-    <row r="20" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="H20" s="24"/>
-      <c r="I20" s="25"/>
-      <c r="J20" s="26"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="H21" s="13"/>
-    </row>
-    <row r="22" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="H22" s="12"/>
-    </row>
-    <row r="23" spans="1:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I18" s="51"/>
+      <c r="J18" s="52"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H19" s="53"/>
+      <c r="I19" s="54"/>
+      <c r="J19" s="55"/>
+    </row>
+    <row r="20" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="H20" s="56"/>
+      <c r="I20" s="57"/>
+      <c r="J20" s="58"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H21" s="12"/>
+    </row>
+    <row r="22" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="H22" s="11"/>
+    </row>
+    <row r="23" spans="1:10" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C23" s="6"/>
     </row>
-    <row r="24" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" t="e">
         <v>#VALUE!</v>
       </c>
@@ -3401,7 +3465,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" t="e">
         <f>NA()</f>
         <v>#N/A</v>
@@ -3418,7 +3482,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" t="e">
         <f>NA()</f>
         <v>#N/A</v>
@@ -3432,7 +3496,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" t="e">
         <f>NA()</f>
         <v>#N/A</v>
@@ -3446,13 +3510,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="D32" t="b">
         <f>ISERROR(C26)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D33" t="b">
         <f>ISERROR(C27)</f>
         <v>1</v>
@@ -3469,22 +3533,34 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{877BF29E-31A1-4B82-8312-1D9EE051B66C}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B490A97C-AF5E-4D84-83BF-8838776215CD}">
   <dimension ref="A1:R19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D24" sqref="D15:H24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.26953125" customWidth="1"/>
-    <col min="4" max="4" width="18.54296875" customWidth="1"/>
-    <col min="8" max="8" width="25.6328125" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" customWidth="1"/>
+    <col min="4" max="4" width="18.5" customWidth="1"/>
+    <col min="8" max="8" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -3501,18 +3577,18 @@
       <c r="H1" t="s">
         <v>39</v>
       </c>
-      <c r="I1" s="27"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="32"/>
-      <c r="O1" s="33"/>
-      <c r="P1" s="34"/>
-      <c r="Q1" s="35"/>
-      <c r="R1" s="36"/>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="I1" s="16"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="23"/>
+      <c r="Q1" s="24"/>
+      <c r="R1" s="25"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -3525,18 +3601,18 @@
       <c r="H2" t="s">
         <v>41</v>
       </c>
-      <c r="I2" s="37"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="39"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="41"/>
-      <c r="N2" s="42"/>
-      <c r="O2" s="43"/>
-      <c r="P2" s="44"/>
-      <c r="Q2" s="45"/>
-      <c r="R2" s="46"/>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="I2" s="26"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="32"/>
+      <c r="P2" s="33"/>
+      <c r="Q2" s="34"/>
+      <c r="R2" s="35"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B3">
         <v>3</v>
       </c>
@@ -3544,7 +3620,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B4">
         <v>4</v>
       </c>
@@ -3552,7 +3628,7 @@
         <v>-4</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B5">
         <v>5</v>
       </c>
@@ -3560,7 +3636,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B6">
         <v>6</v>
       </c>
@@ -3571,40 +3647,40 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B7">
         <v>7</v>
       </c>
       <c r="H7" t="s">
         <v>40</v>
       </c>
-      <c r="I7" s="47"/>
-      <c r="J7" s="48"/>
-      <c r="K7" s="49"/>
-      <c r="L7" s="50"/>
-      <c r="M7" s="51"/>
-      <c r="N7" s="52"/>
-      <c r="O7" s="53"/>
-      <c r="P7" s="54"/>
-      <c r="Q7" s="55"/>
-      <c r="R7" s="56"/>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="I7" s="36"/>
+      <c r="J7" s="37"/>
+      <c r="K7" s="38"/>
+      <c r="L7" s="39"/>
+      <c r="M7" s="40"/>
+      <c r="N7" s="41"/>
+      <c r="O7" s="42"/>
+      <c r="P7" s="43"/>
+      <c r="Q7" s="44"/>
+      <c r="R7" s="45"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B8">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B9">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>1</v>
       </c>
@@ -3612,7 +3688,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2</v>
       </c>
@@ -3620,7 +3696,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>3</v>
       </c>
@@ -3681,16 +3757,16 @@
   <dimension ref="A3:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="H25" sqref="D18:H25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>31</v>
       </c>
@@ -3698,83 +3774,83 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4">
         <v>1980</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="10" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5">
         <v>1980</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="11" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6">
         <v>1980</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7">
         <v>1980</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" s="10" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B8">
         <v>1980</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" s="11" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="9">
+      <c r="B9">
         <v>1980</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="9">
+      <c r="B10">
         <v>1975</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" s="10" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="9">
+      <c r="B11">
         <v>1975</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" s="11" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="9">
+      <c r="B12">
         <v>1975</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="9">
+      <c r="B13">
         <v>5935</v>
       </c>
     </row>
@@ -3791,9 +3867,9 @@
       <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>1</v>
       </c>
@@ -3813,7 +3889,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2</v>
       </c>
@@ -3833,7 +3909,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>3</v>
       </c>
@@ -3853,7 +3929,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>4</v>
       </c>
@@ -3873,7 +3949,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>5</v>
       </c>
@@ -3912,9 +3988,9 @@
       <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -3928,7 +4004,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -3942,7 +4018,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -3956,7 +4032,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -3986,9 +4062,9 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>1</v>
       </c>
@@ -3996,7 +4072,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2</v>
       </c>
@@ -4004,7 +4080,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>3</v>
       </c>
@@ -4023,36 +4099,36 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="D15" sqref="D9:F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="39.81640625" customWidth="1"/>
+    <col min="1" max="1" width="39.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="15" t="s">
+    <row r="6" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="14" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:2" s="16" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="16" t="s">
+    <row r="7" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="15" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B11" s="15" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B11" s="14" t="s">
         <v>38</v>
       </c>
     </row>
@@ -4063,13 +4139,178 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{877BF29E-31A1-4B82-8312-1D9EE051B66C}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73C1FDB6-89EB-0F47-9151-342FE6A4B95C}">
+  <dimension ref="A1:S30"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" sqref="A1:B2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="10.83203125" style="46"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:16" s="47" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="2:16" s="47" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="2:16" s="47" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="47" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>43</v>
+      </c>
+      <c r="P4" s="20"/>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="P5" s="20"/>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="P6" s="20"/>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="P7" s="20"/>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="P8" s="20"/>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="P9" s="20"/>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="P10" s="20"/>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="P11" s="20"/>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="P12" s="20"/>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="I13">
+        <f>1+1</f>
+        <v>2</v>
+      </c>
+      <c r="P13" s="20"/>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="P14" s="20"/>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="P15" s="20"/>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="P16" s="20"/>
+    </row>
+    <row r="17" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="P17" s="20"/>
+    </row>
+    <row r="18" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="P18" s="20"/>
+    </row>
+    <row r="19" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="P19" s="20"/>
+    </row>
+    <row r="20" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="P20" s="20"/>
+    </row>
+    <row r="21" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="C21" s="48"/>
+      <c r="D21" s="48"/>
+      <c r="E21" s="48"/>
+      <c r="F21" s="48"/>
+      <c r="G21" s="48"/>
+      <c r="H21" s="48"/>
+      <c r="I21" s="48"/>
+      <c r="J21" s="48"/>
+      <c r="K21" s="48"/>
+      <c r="L21" s="48"/>
+      <c r="M21" s="48"/>
+      <c r="N21" s="48"/>
+      <c r="O21" s="48"/>
+      <c r="P21" s="20"/>
+      <c r="Q21" s="48"/>
+      <c r="R21" s="48"/>
+      <c r="S21" s="48"/>
+    </row>
+    <row r="22" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="P22" s="20"/>
+    </row>
+    <row r="23" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="P23" s="20"/>
+    </row>
+    <row r="24" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="P24" s="20"/>
+    </row>
+    <row r="25" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="P25" s="20"/>
+    </row>
+    <row r="26" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="P26" s="20"/>
+    </row>
+    <row r="27" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="P27" s="20"/>
+    </row>
+    <row r="28" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="P28" s="20"/>
+    </row>
+    <row r="29" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="P29" s="20"/>
+    </row>
+    <row r="30" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="P30" s="20"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A98731A-1BE1-2943-936B-6BF79B02CD3E}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="8260" ySplit="3440"/>
+      <selection activeCell="C2" sqref="C2"/>
+      <selection pane="topRight" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
+      <selection pane="bottomRight" activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
UPDATE: Parses selected row/column/range and selected sheet (#67)
* FIX: Update to Rust 1.78.0

* UPDATE: Parses selected row/column/range and selected sheet
</commit_message>
<xml_diff>
--- a/xlsx/tests/example.xlsx
+++ b/xlsx/tests/example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20368"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nhatcher/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1735EC9-FFED-419C-B07A-CFF93E3E2AA9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E08456FE-9C8A-184E-905A-1DA5ECA32BA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="6020" windowHeight="50" activeTab="2" xr2:uid="{94D94FA5-4B40-4032-9EB1-15E3426A29B1}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" activeTab="8" xr2:uid="{94D94FA5-4B40-4032-9EB1-15E3426A29B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,9 @@
     <sheet name="Table" sheetId="7" r:id="rId6"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId7"/>
     <sheet name="Created fourth" sheetId="4" r:id="rId8"/>
-    <sheet name="Hidden" sheetId="5" state="hidden" r:id="rId9"/>
+    <sheet name="Frozen" sheetId="10" r:id="rId9"/>
+    <sheet name="Split" sheetId="11" r:id="rId10"/>
+    <sheet name="Hidden" sheetId="5" state="hidden" r:id="rId11"/>
   </sheets>
   <definedNames>
     <definedName name="answer" localSheetId="4">shared!$G$5</definedName>
@@ -32,11 +34,22 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId10"/>
+    <pivotCache cacheId="2" r:id="rId12"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -56,7 +69,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>nicol:</t>
         </r>
@@ -65,7 +78,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 This cell has bold! Text. Náguara!</t>
@@ -78,21 +91,30 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>nicol:</t>
         </r>
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-There is a coment here, you know
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">There is a coment here, you know
 </t>
         </r>
       </text>
@@ -105,7 +127,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>nicol:</t>
         </r>
@@ -114,7 +136,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 New comment</t>
@@ -129,7 +151,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>nicol:</t>
         </r>
@@ -138,7 +160,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 There is a </t>
@@ -158,7 +180,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> here.
 </t>
@@ -193,7 +215,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="47">
   <si>
     <t>A string</t>
   </si>
@@ -344,12 +366,27 @@
   <si>
     <t>With a tint</t>
   </si>
+  <si>
+    <t>Corner</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>B4</t>
+  </si>
+  <si>
+    <t>as</t>
+  </si>
+  <si>
+    <t>df</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -406,14 +443,14 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -437,20 +474,27 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="5" tint="-0.24994659260841701"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="36">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -659,6 +703,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="14">
     <border>
@@ -818,9 +880,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -832,7 +894,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
@@ -842,8 +903,41 @@
     <xf numFmtId="0" fontId="11" fillId="7" borderId="3" xfId="2"/>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="4" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="5" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="3" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="3" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -874,36 +968,6 @@
     <xf numFmtId="0" fontId="11" fillId="7" borderId="13" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="27" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="30" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Input" xfId="2" builtinId="20"/>
@@ -935,7 +999,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1276,7 +1340,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2827,7 +2891,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D44FF134-98CE-4CDD-8BF9-3EB1A09B9FAE}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D44FF134-98CE-4CDD-8BF9-3EB1A09B9FAE}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B13" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" showAll="0">
@@ -2924,9 +2988,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2964,7 +3028,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -3070,7 +3134,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3212,7 +3276,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3223,17 +3287,17 @@
   <dimension ref="A1:O33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="E13" sqref="E13:N20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="5" width="38.26953125" customWidth="1"/>
-    <col min="6" max="6" width="9.1796875" style="1"/>
+    <col min="5" max="5" width="38.33203125" customWidth="1"/>
+    <col min="6" max="6" width="9.1640625" style="1"/>
     <col min="8" max="8" width="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3254,7 +3318,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>222</v>
       </c>
@@ -3272,7 +3336,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B3">
         <f>A3</f>
         <v>0</v>
@@ -3288,44 +3352,44 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="I6" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="13" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="K7" s="17" t="s">
+    <row r="7" spans="1:15" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K7" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="L7" s="17"/>
-    </row>
-    <row r="8" spans="1:15" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="K8" s="17"/>
-      <c r="L8" s="17"/>
+      <c r="L7" s="49"/>
+    </row>
+    <row r="8" spans="1:15" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K8" s="49"/>
+      <c r="L8" s="49"/>
       <c r="N8" s="3"/>
       <c r="O8" s="3"/>
     </row>
-    <row r="9" spans="1:15" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" ht="29.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E9" t="s">
         <v>12</v>
       </c>
-      <c r="K9" s="17"/>
-      <c r="L9" s="17"/>
+      <c r="K9" s="49"/>
+      <c r="L9" s="49"/>
       <c r="N9" s="3" t="s">
         <v>8</v>
       </c>
       <c r="O9" s="3"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="K10" s="17"/>
-      <c r="L10" s="17"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="K10" s="49"/>
+      <c r="L10" s="49"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C14" t="s">
         <v>9</v>
       </c>
@@ -3334,24 +3398,24 @@
         <v>quantum</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="21" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="K15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2</v>
       </c>
-      <c r="H16" s="12"/>
-    </row>
-    <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H16" s="11"/>
+    </row>
+    <row r="17" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>6</v>
       </c>
-      <c r="H17" s="14"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H17" s="13"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>7</v>
       </c>
@@ -3359,36 +3423,36 @@
         <f>SUM(numbers)</f>
         <v>15</v>
       </c>
-      <c r="H18" s="18">
+      <c r="H18" s="50">
         <v>1</v>
       </c>
-      <c r="I18" s="19"/>
-      <c r="J18" s="20"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="H19" s="21"/>
-      <c r="I19" s="22"/>
-      <c r="J19" s="23"/>
-    </row>
-    <row r="20" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="H20" s="24"/>
-      <c r="I20" s="25"/>
-      <c r="J20" s="26"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="H21" s="13"/>
-    </row>
-    <row r="22" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="H22" s="12"/>
-    </row>
-    <row r="23" spans="1:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I18" s="51"/>
+      <c r="J18" s="52"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H19" s="53"/>
+      <c r="I19" s="54"/>
+      <c r="J19" s="55"/>
+    </row>
+    <row r="20" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="H20" s="56"/>
+      <c r="I20" s="57"/>
+      <c r="J20" s="58"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H21" s="12"/>
+    </row>
+    <row r="22" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="H22" s="11"/>
+    </row>
+    <row r="23" spans="1:10" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C23" s="6"/>
     </row>
-    <row r="24" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" t="e">
         <v>#VALUE!</v>
       </c>
@@ -3401,7 +3465,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" t="e">
         <f>NA()</f>
         <v>#N/A</v>
@@ -3418,7 +3482,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" t="e">
         <f>NA()</f>
         <v>#N/A</v>
@@ -3432,7 +3496,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" t="e">
         <f>NA()</f>
         <v>#N/A</v>
@@ -3446,13 +3510,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="D32" t="b">
         <f>ISERROR(C26)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D33" t="b">
         <f>ISERROR(C27)</f>
         <v>1</v>
@@ -3469,22 +3533,34 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{877BF29E-31A1-4B82-8312-1D9EE051B66C}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B490A97C-AF5E-4D84-83BF-8838776215CD}">
   <dimension ref="A1:R19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D24" sqref="D15:H24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.26953125" customWidth="1"/>
-    <col min="4" max="4" width="18.54296875" customWidth="1"/>
-    <col min="8" max="8" width="25.6328125" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" customWidth="1"/>
+    <col min="4" max="4" width="18.5" customWidth="1"/>
+    <col min="8" max="8" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -3501,18 +3577,18 @@
       <c r="H1" t="s">
         <v>39</v>
       </c>
-      <c r="I1" s="27"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="32"/>
-      <c r="O1" s="33"/>
-      <c r="P1" s="34"/>
-      <c r="Q1" s="35"/>
-      <c r="R1" s="36"/>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="I1" s="16"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="23"/>
+      <c r="Q1" s="24"/>
+      <c r="R1" s="25"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -3525,18 +3601,18 @@
       <c r="H2" t="s">
         <v>41</v>
       </c>
-      <c r="I2" s="37"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="39"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="41"/>
-      <c r="N2" s="42"/>
-      <c r="O2" s="43"/>
-      <c r="P2" s="44"/>
-      <c r="Q2" s="45"/>
-      <c r="R2" s="46"/>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="I2" s="26"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="32"/>
+      <c r="P2" s="33"/>
+      <c r="Q2" s="34"/>
+      <c r="R2" s="35"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B3">
         <v>3</v>
       </c>
@@ -3544,7 +3620,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B4">
         <v>4</v>
       </c>
@@ -3552,7 +3628,7 @@
         <v>-4</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B5">
         <v>5</v>
       </c>
@@ -3560,7 +3636,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B6">
         <v>6</v>
       </c>
@@ -3571,40 +3647,40 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B7">
         <v>7</v>
       </c>
       <c r="H7" t="s">
         <v>40</v>
       </c>
-      <c r="I7" s="47"/>
-      <c r="J7" s="48"/>
-      <c r="K7" s="49"/>
-      <c r="L7" s="50"/>
-      <c r="M7" s="51"/>
-      <c r="N7" s="52"/>
-      <c r="O7" s="53"/>
-      <c r="P7" s="54"/>
-      <c r="Q7" s="55"/>
-      <c r="R7" s="56"/>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="I7" s="36"/>
+      <c r="J7" s="37"/>
+      <c r="K7" s="38"/>
+      <c r="L7" s="39"/>
+      <c r="M7" s="40"/>
+      <c r="N7" s="41"/>
+      <c r="O7" s="42"/>
+      <c r="P7" s="43"/>
+      <c r="Q7" s="44"/>
+      <c r="R7" s="45"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B8">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B9">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>1</v>
       </c>
@@ -3612,7 +3688,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2</v>
       </c>
@@ -3620,7 +3696,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>3</v>
       </c>
@@ -3681,16 +3757,16 @@
   <dimension ref="A3:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="H25" sqref="D18:H25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>31</v>
       </c>
@@ -3698,83 +3774,83 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4">
         <v>1980</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="10" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5">
         <v>1980</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="11" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6">
         <v>1980</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7">
         <v>1980</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" s="10" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B8">
         <v>1980</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" s="11" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="9">
+      <c r="B9">
         <v>1980</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="9">
+      <c r="B10">
         <v>1975</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" s="10" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="9">
+      <c r="B11">
         <v>1975</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" s="11" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="9">
+      <c r="B12">
         <v>1975</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="9">
+      <c r="B13">
         <v>5935</v>
       </c>
     </row>
@@ -3791,9 +3867,9 @@
       <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>1</v>
       </c>
@@ -3813,7 +3889,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2</v>
       </c>
@@ -3833,7 +3909,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>3</v>
       </c>
@@ -3853,7 +3929,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>4</v>
       </c>
@@ -3873,7 +3949,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>5</v>
       </c>
@@ -3912,9 +3988,9 @@
       <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -3928,7 +4004,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -3942,7 +4018,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -3956,7 +4032,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -3986,9 +4062,9 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>1</v>
       </c>
@@ -3996,7 +4072,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2</v>
       </c>
@@ -4004,7 +4080,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>3</v>
       </c>
@@ -4023,36 +4099,36 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="D15" sqref="D9:F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="39.81640625" customWidth="1"/>
+    <col min="1" max="1" width="39.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="15" t="s">
+    <row r="6" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="14" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:2" s="16" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="16" t="s">
+    <row r="7" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="15" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B11" s="15" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B11" s="14" t="s">
         <v>38</v>
       </c>
     </row>
@@ -4063,13 +4139,178 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{877BF29E-31A1-4B82-8312-1D9EE051B66C}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73C1FDB6-89EB-0F47-9151-342FE6A4B95C}">
+  <dimension ref="A1:S30"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" sqref="A1:B2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="10.83203125" style="46"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:16" s="47" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="2:16" s="47" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="2:16" s="47" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="47" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>43</v>
+      </c>
+      <c r="P4" s="20"/>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="P5" s="20"/>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="P6" s="20"/>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="P7" s="20"/>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="P8" s="20"/>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="P9" s="20"/>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="P10" s="20"/>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="P11" s="20"/>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="P12" s="20"/>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="I13">
+        <f>1+1</f>
+        <v>2</v>
+      </c>
+      <c r="P13" s="20"/>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="P14" s="20"/>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="P15" s="20"/>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="P16" s="20"/>
+    </row>
+    <row r="17" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="P17" s="20"/>
+    </row>
+    <row r="18" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="P18" s="20"/>
+    </row>
+    <row r="19" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="P19" s="20"/>
+    </row>
+    <row r="20" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="P20" s="20"/>
+    </row>
+    <row r="21" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="C21" s="48"/>
+      <c r="D21" s="48"/>
+      <c r="E21" s="48"/>
+      <c r="F21" s="48"/>
+      <c r="G21" s="48"/>
+      <c r="H21" s="48"/>
+      <c r="I21" s="48"/>
+      <c r="J21" s="48"/>
+      <c r="K21" s="48"/>
+      <c r="L21" s="48"/>
+      <c r="M21" s="48"/>
+      <c r="N21" s="48"/>
+      <c r="O21" s="48"/>
+      <c r="P21" s="20"/>
+      <c r="Q21" s="48"/>
+      <c r="R21" s="48"/>
+      <c r="S21" s="48"/>
+    </row>
+    <row r="22" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="P22" s="20"/>
+    </row>
+    <row r="23" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="P23" s="20"/>
+    </row>
+    <row r="24" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="P24" s="20"/>
+    </row>
+    <row r="25" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="P25" s="20"/>
+    </row>
+    <row r="26" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="P26" s="20"/>
+    </row>
+    <row r="27" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="P27" s="20"/>
+    </row>
+    <row r="28" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="P28" s="20"/>
+    </row>
+    <row r="29" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="P29" s="20"/>
+    </row>
+    <row r="30" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="P30" s="20"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A98731A-1BE1-2943-936B-6BF79B02CD3E}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="8260" ySplit="3440"/>
+      <selection activeCell="C2" sqref="C2"/>
+      <selection pane="topRight" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
+      <selection pane="bottomRight" activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>